<commit_message>
Update - Correction of Aprendendo.xlsx content
</commit_message>
<xml_diff>
--- a/Aprendendo.xlsx
+++ b/Aprendendo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faell\OneDrive\Documentos\GitHub\EnglishBotPrivate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faell\OneDrive\Documentos\GitHub\EnglishBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A8C24A-A120-40F2-A0F4-3E91B0874BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9053C71B-0244-4E0B-974C-CC612D5FF7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{D471F43C-4ACE-4E09-8D25-8F9F710D45A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D471F43C-4ACE-4E09-8D25-8F9F710D45A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeros" sheetId="1" r:id="rId1"/>
@@ -128,6 +128,9 @@
     <t>Conteudo</t>
   </si>
   <si>
+    <t>three</t>
+  </si>
+  <si>
     <t>Os números em inglês possuem uma regra básica para sua formação. Até o vigésimo número(20) possuem um nome 'fixo', como visto abaixo:
 0 - Zero
 1 - One
@@ -151,8 +154,8 @@
 19 - Nineteen
 20 - Twenty
 A partir no número 20, os outros são formados com base nos 20 primeiro, mudando somente a dezena, exemplo:
-O número 21 é formado juntando a dezena do 20(Twenty) + o número específico ( 1 - One ) - Twenty-one
- O número 22 - Twenty-two
+O número 21 é formado juntando a dezena do 20(Twenty) + o número específico ( 1 - One ) - Twenty one
+ O número 22 - Twenty two
 Esta regra segue para todos os outros números até 99, segue a dezena de cada número:
 30 - Thirty
 40 - Forty
@@ -165,11 +168,11 @@
 As centenas são construídas seguindo o padrão: 
 número específico( 1,2,3,4...) + hundred(representa a centena) + dezena por extenso(mesma escrita dos números de 1 a 99)
 Exemplo:
-100 - One(representa o número 1 que vem em primeiro) + hundred - One-hundred (Como é 100, não possui os números especificos da dezena)
-101 - One(representa o número 1 que vem em primeiro) + hundred + one(número da dezena) - One-hundred and one
-105 - One(representa o número 1 que vem em primeiro) + hundred + five(número da dezena) - One-hundred and five
-112 - One(representa o número 1 que vem em primeiro) + hundred + twelve(número da dezena) - One-hundred and twelve
-135 - One(representa o número 1 que vem em primeiro) + hundred + thirty-five(número da dezena) - One-hundred and thirty-five
+100 - One(representa o número 1 que vem em primeiro) + hundred - One hundred (Como é 100, não possui os números especificos da dezena)
+101 - One(representa o número 1 que vem em primeiro) + hundred + one(número da dezena) - One hundred one
+105 - One(representa o número 1 que vem em primeiro) + hundred + five(número da dezena) - One hundred five
+112 - One(representa o número 1 que vem em primeiro) + hundred + twelve(número da dezena) - One hundred twelve
+135 - One(representa o número 1 que vem em primeiro) + hundred + thirty-five(número da dezena) - One hundred thirty five
 Como anteriormente essa regra se repete para as outras centenas:
 100 - One
 200 - Two
@@ -177,17 +180,14 @@
 400, 500, 600...
 Para a casa dos milhares a regra segue o mesmo padrão das centenas, porém acrescentando a casa do milhar antes:
 Numero específico  + thousand(representa o milhar) + centena por extenso + dezena por extenso
-1000 - One-thousand
-1005 - One-thounsand and five
-1055 - One-thousand and fifty-five
-1234 - One-thounsand and two-hundred and thirty-four
+1000 - One thousand
+1005 - One thounsand five
+1055 - One thousand fifty five
+1234 - One thounsand two hundred thirty four
 E a regra se repete para os demais, mudando apenas a nomeação do primeiro número:
-2400 - TWO-thousand and four-hundred
-3556 - THREE-thousand and five-hundred and fifty-six
-4000 - Four-thousand</t>
-  </si>
-  <si>
-    <t>three</t>
+2400 - TWO thousand four hundred
+3556 - THREE thousand five hundred fifty six
+4000 - Four thousand</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADAD5F3-41A3-4E88-80DD-A3EC125A2FC6}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update - Code Hash
</commit_message>
<xml_diff>
--- a/Aprendendo.xlsx
+++ b/Aprendendo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faell\OneDrive\Documentos\GitHub\EnglishBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9053C71B-0244-4E0B-974C-CC612D5FF7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440EB75F-A96F-4170-9B13-47D355D472E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D471F43C-4ACE-4E09-8D25-8F9F710D45A5}"/>
   </bookViews>
@@ -185,8 +185,8 @@
 1055 - One thousand fifty five
 1234 - One thounsand two hundred thirty four
 E a regra se repete para os demais, mudando apenas a nomeação do primeiro número:
-2400 - TWO thousand four hundred
-3556 - THREE thousand five hundred fifty six
+2400 - TWO thousand and four-hundred
+3556 - THREE thousand and five-hundred and fifty-six
 4000 - Four thousand</t>
   </si>
 </sst>

</xml_diff>